<commit_message>
done with multiple ports
</commit_message>
<xml_diff>
--- a/data/committed_cargoes.xlsx
+++ b/data/committed_cargoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Y3S2\SMU\cargill_datathon_freight_calculator_chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91775207-2C48-4488-A858-AD35847BB547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCB1288-60EC-41C5-89AD-162E50FB5E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{16041185-FF1A-44AC-8CA7-254566FB0610}"/>
+    <workbookView xWindow="48" yWindow="288" windowWidth="22992" windowHeight="13392" xr2:uid="{16041185-FF1A-44AC-8CA7-254566FB0610}"/>
   </bookViews>
   <sheets>
     <sheet name="market_vessel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>start_route</t>
   </si>
@@ -143,12 +143,6 @@
     <t>discharge_port1</t>
   </si>
   <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>Far East</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Anchorage Loading</t>
   </si>
   <si>
@@ -180,6 +174,15 @@
   </si>
   <si>
     <t>total_port_cost</t>
+  </si>
+  <si>
+    <t>TIANJIN</t>
+  </si>
+  <si>
+    <t>RIZHAO</t>
+  </si>
+  <si>
+    <t>discharge_port3</t>
   </si>
 </sst>
 </file>
@@ -1042,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F04A88-483C-4287-871A-7E299D864160}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1053,16 +1056,16 @@
     <col min="1" max="9" width="38.33203125" customWidth="1"/>
     <col min="10" max="10" width="53.77734375" customWidth="1"/>
     <col min="11" max="16" width="38.33203125" customWidth="1"/>
-    <col min="17" max="18" width="69.6640625" customWidth="1"/>
-    <col min="19" max="24" width="38.33203125" customWidth="1"/>
+    <col min="17" max="19" width="69.6640625" customWidth="1"/>
+    <col min="20" max="25" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
@@ -1098,7 +1101,7 @@
         <v>30</v>
       </c>
       <c r="N1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
@@ -1113,28 +1116,31 @@
         <v>34</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
-      <c r="W1" t="s">
-        <v>48</v>
-      </c>
       <c r="X1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K2" s="2">
         <v>46114</v>
@@ -1175,7 +1181,7 @@
         <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O2">
         <v>30000</v>
@@ -1184,26 +1190,26 @@
         <v>12</v>
       </c>
       <c r="Q2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2">
+        <v>47</v>
+      </c>
+      <c r="T2">
         <v>25000</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>12</v>
       </c>
-      <c r="W2">
-        <f>U2+V2</f>
+      <c r="X2">
+        <f>V2+W2</f>
         <v>0</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1244,7 +1250,7 @@
         <v>9</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O3">
         <v>80000</v>
@@ -1253,29 +1259,29 @@
         <v>12</v>
       </c>
       <c r="Q3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3">
+        <v>42</v>
+      </c>
+      <c r="T3">
         <v>30000</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>24</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>260000</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>120000</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W4" si="0">U3+V3</f>
+      <c r="X3">
+        <f t="shared" ref="X3:X4" si="0">V3+W3</f>
         <v>380000</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1301,10 +1307,10 @@
         <v>0.1</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K4" s="2">
         <v>46113</v>
@@ -1316,7 +1322,7 @@
         <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O4">
         <v>60000</v>
@@ -1325,28 +1331,31 @@
         <v>6</v>
       </c>
       <c r="Q4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4">
+        <v>48</v>
+      </c>
+      <c r="S4" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4">
         <v>30000</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>24</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>75000</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>90000</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <f t="shared" si="0"/>
         <v>165000</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>